<commit_message>
Added excel file, matlab code and screenshots
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,8 +473,8 @@
       <c r="D5" s="2">
         <v>1.6977100000000001</v>
       </c>
-      <c r="E5" s="1">
-        <v>168644786</v>
+      <c r="E5" s="2">
+        <v>168.64478600000001</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>

</xml_diff>